<commit_message>
Added documentation for Richmond and VABeach rental prices data sets
</commit_message>
<xml_diff>
--- a/cs5010_Dict_DRAFTv2_100720.xlsx
+++ b/cs5010_Dict_DRAFTv2_100720.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie\Documents\MSDS Program\CS 5010\CS Project\LifeOfBrian-USHousing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana McSpadden\Documents\UVaCode\Python\LifeOfBrian-USHousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE67748A-B2F8-4507-A4DD-E36356B1022B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EBD54B-2B60-43FC-BBBD-84C149BC0474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
+    <workbookView xWindow="1860" yWindow="672" windowWidth="20316" windowHeight="11352" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="125">
   <si>
     <t>Source</t>
   </si>
@@ -361,6 +361,45 @@
   </si>
   <si>
     <t>percOfTotal</t>
+  </si>
+  <si>
+    <t>median_rent_price</t>
+  </si>
+  <si>
+    <t>Richmond, VA median rent price for year</t>
+  </si>
+  <si>
+    <t>location_name == Richmond, VA</t>
+  </si>
+  <si>
+    <t>https://www.deptofnumbers.com/rent/virginia/richmond/</t>
+  </si>
+  <si>
+    <t>web scraped to CSV</t>
+  </si>
+  <si>
+    <t>Dept of Numbers</t>
+  </si>
+  <si>
+    <t>median gross rent</t>
+  </si>
+  <si>
+    <t>mean_rent_price</t>
+  </si>
+  <si>
+    <t>Richmond, VA mean rent price for year</t>
+  </si>
+  <si>
+    <t>mean gross rent</t>
+  </si>
+  <si>
+    <t>Virginia Beach, VA median rent price for year</t>
+  </si>
+  <si>
+    <t>Virginia Beach, VA mean rent price for year</t>
+  </si>
+  <si>
+    <t>location_name == Virginia Beach, VA</t>
   </si>
 </sst>
 </file>
@@ -791,43 +830,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE930BE5-76EF-4DE3-A62A-9FA65577EC5F}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
-    <col min="16" max="21" width="15.85546875" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="16" max="21" width="15.88671875" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.109375" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" customWidth="1"/>
     <col min="27" max="27" width="23" customWidth="1"/>
-    <col min="28" max="28" width="20.42578125" customWidth="1"/>
-    <col min="29" max="29" width="18.7109375" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" customWidth="1"/>
+    <col min="28" max="28" width="20.44140625" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" customWidth="1"/>
+    <col min="30" max="30" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
@@ -836,10 +875,10 @@
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -931,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -1023,7 +1062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1115,7 +1154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -1207,7 +1246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1299,7 +1338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1391,7 +1430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -1483,7 +1522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -1575,7 +1614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -1667,7 +1706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -1759,7 +1798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>10</v>
       </c>
@@ -1851,7 +1890,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -1943,7 +1982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -2035,7 +2074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -2123,7 +2162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>14</v>
       </c>
@@ -2215,7 +2254,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>15</v>
       </c>
@@ -2307,7 +2346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -2399,7 +2438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>17</v>
       </c>
@@ -2491,7 +2530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>18</v>
       </c>
@@ -2583,7 +2622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -2675,7 +2714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>20</v>
       </c>
@@ -2767,7 +2806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>21</v>
       </c>
@@ -2859,135 +2898,375 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0</v>
+      </c>
+      <c r="J26" s="8">
+        <v>0</v>
+      </c>
+      <c r="K26" s="8">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8">
+        <v>2006</v>
+      </c>
+      <c r="M26" s="8">
+        <v>2017</v>
+      </c>
+      <c r="N26" s="8">
+        <v>0</v>
+      </c>
+      <c r="O26" s="8">
+        <v>0</v>
+      </c>
+      <c r="P26" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>0</v>
+      </c>
+      <c r="R26" s="8">
+        <v>1</v>
+      </c>
+      <c r="S26" s="8">
+        <v>0</v>
+      </c>
+      <c r="T26" s="8">
+        <v>0</v>
+      </c>
+      <c r="U26" s="8">
+        <v>0</v>
+      </c>
+      <c r="V26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="W26" s="8">
+        <v>944</v>
+      </c>
+      <c r="X26" s="8">
+        <v>1060</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z26" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC26" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD26" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="8"/>
-      <c r="AB27" s="8"/>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="8"/>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>23</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0</v>
+      </c>
+      <c r="L27" s="8">
+        <v>2006</v>
+      </c>
+      <c r="M27" s="8">
+        <v>2017</v>
+      </c>
+      <c r="N27" s="8">
+        <v>0</v>
+      </c>
+      <c r="O27" s="8">
+        <v>0</v>
+      </c>
+      <c r="P27" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>0</v>
+      </c>
+      <c r="R27" s="8">
+        <v>1</v>
+      </c>
+      <c r="S27" s="8">
+        <v>0</v>
+      </c>
+      <c r="T27" s="8">
+        <v>0</v>
+      </c>
+      <c r="U27" s="8">
+        <v>0</v>
+      </c>
+      <c r="V27" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="W27" s="8">
+        <v>922</v>
+      </c>
+      <c r="X27" s="8">
+        <v>1059</v>
+      </c>
+      <c r="Y27" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD27" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="8"/>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="8"/>
-      <c r="AD28" s="8"/>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0</v>
+      </c>
+      <c r="L28" s="8">
+        <v>2006</v>
+      </c>
+      <c r="M28" s="8">
+        <v>2017</v>
+      </c>
+      <c r="N28" s="8">
+        <v>0</v>
+      </c>
+      <c r="O28" s="8">
+        <v>0</v>
+      </c>
+      <c r="P28" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>0</v>
+      </c>
+      <c r="R28" s="8">
+        <v>1</v>
+      </c>
+      <c r="S28" s="8">
+        <v>0</v>
+      </c>
+      <c r="T28" s="8">
+        <v>0</v>
+      </c>
+      <c r="U28" s="8">
+        <v>0</v>
+      </c>
+      <c r="V28" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="W28" s="8">
+        <v>944</v>
+      </c>
+      <c r="X28" s="8">
+        <v>1060</v>
+      </c>
+      <c r="Y28" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z28" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB28" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC28" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD28" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="8"/>
-      <c r="AC29" s="8"/>
-      <c r="AD29" s="8"/>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>23</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0</v>
+      </c>
+      <c r="K29" s="8">
+        <v>0</v>
+      </c>
+      <c r="L29" s="8">
+        <v>2006</v>
+      </c>
+      <c r="M29" s="8">
+        <v>2017</v>
+      </c>
+      <c r="N29" s="8">
+        <v>0</v>
+      </c>
+      <c r="O29" s="8">
+        <v>0</v>
+      </c>
+      <c r="P29" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>0</v>
+      </c>
+      <c r="R29" s="8">
+        <v>1</v>
+      </c>
+      <c r="S29" s="8">
+        <v>0</v>
+      </c>
+      <c r="T29" s="8">
+        <v>0</v>
+      </c>
+      <c r="U29" s="8">
+        <v>0</v>
+      </c>
+      <c r="V29" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="W29" s="8">
+        <v>922</v>
+      </c>
+      <c r="X29" s="8">
+        <v>1059</v>
+      </c>
+      <c r="Y29" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC29" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD29" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="13"/>
@@ -3019,7 +3298,7 @@
       <c r="AC30" s="8"/>
       <c r="AD30" s="8"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="13"/>
@@ -3051,7 +3330,7 @@
       <c r="AC31" s="8"/>
       <c r="AD31" s="8"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="13"/>
@@ -3083,7 +3362,7 @@
       <c r="AC32" s="8"/>
       <c r="AD32" s="8"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="13"/>
@@ -3115,7 +3394,7 @@
       <c r="AC33" s="8"/>
       <c r="AD33" s="8"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="13"/>
@@ -3147,7 +3426,7 @@
       <c r="AC34" s="8"/>
       <c r="AD34" s="8"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="13"/>

</xml_diff>

<commit_message>
inflation 1995 ipynb work
</commit_message>
<xml_diff>
--- a/cs5010_Dict_DRAFTv2_100720.xlsx
+++ b/cs5010_Dict_DRAFTv2_100720.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana McSpadden\Documents\UVaCode\Python\LifeOfBrian-USHousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EBD54B-2B60-43FC-BBBD-84C149BC0474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B9BB83-E7FE-4D79-A3B4-3B5023C1FC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="672" windowWidth="20316" windowHeight="11352" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
+    <workbookView xWindow="34905" yWindow="2460" windowWidth="20205" windowHeight="11355" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="134">
   <si>
     <t>Source</t>
   </si>
@@ -400,6 +409,33 @@
   </si>
   <si>
     <t>location_name == Virginia Beach, VA</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Dollar amount in 1995 dollars</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>https://www.in2013dollars.com/us/inflation/1995</t>
+  </si>
+  <si>
+    <t>in2013Dollars.com from Bureau Of Labor Statistics</t>
+  </si>
+  <si>
+    <t>inflation rate</t>
+  </si>
+  <si>
+    <t>year over year inflation rate</t>
+  </si>
+  <si>
+    <t>cumulative</t>
+  </si>
+  <si>
+    <t>cumulative from 1995 inflation rate</t>
   </si>
 </sst>
 </file>
@@ -479,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -513,6 +549,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,9 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE930BE5-76EF-4DE3-A62A-9FA65577EC5F}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W28" sqref="W28"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD31" sqref="AD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3267,100 +3304,280 @@
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="8"/>
-      <c r="AD30" s="8"/>
+      <c r="A30" s="8">
+        <v>24</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8">
+        <v>1995</v>
+      </c>
+      <c r="M30" s="8">
+        <v>2020</v>
+      </c>
+      <c r="N30" s="8">
+        <v>1</v>
+      </c>
+      <c r="O30" s="8">
+        <v>0</v>
+      </c>
+      <c r="P30" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>0</v>
+      </c>
+      <c r="R30" s="8">
+        <v>0</v>
+      </c>
+      <c r="S30" s="8">
+        <v>0</v>
+      </c>
+      <c r="T30" s="8">
+        <v>0</v>
+      </c>
+      <c r="U30" s="8">
+        <v>0</v>
+      </c>
+      <c r="V30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="W30" s="8">
+        <v>1</v>
+      </c>
+      <c r="X30" s="8">
+        <v>1.71</v>
+      </c>
+      <c r="Y30" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z30" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB30" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD30" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-      <c r="AB31" s="8"/>
-      <c r="AC31" s="8"/>
-      <c r="AD31" s="8"/>
+      <c r="A31" s="8">
+        <v>25</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0</v>
+      </c>
+      <c r="L31" s="8">
+        <v>1995</v>
+      </c>
+      <c r="M31" s="8">
+        <v>2020</v>
+      </c>
+      <c r="N31" s="8">
+        <v>1</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0</v>
+      </c>
+      <c r="R31" s="8">
+        <v>0</v>
+      </c>
+      <c r="S31" s="8">
+        <v>0</v>
+      </c>
+      <c r="T31" s="8">
+        <v>0</v>
+      </c>
+      <c r="U31" s="8">
+        <v>0</v>
+      </c>
+      <c r="V31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="W31" s="8">
+        <v>0</v>
+      </c>
+      <c r="X31" s="8">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="Y31" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z31" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC31" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD31" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
-      <c r="AD32" s="8"/>
+      <c r="A32" s="8">
+        <v>26</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0</v>
+      </c>
+      <c r="L32" s="8">
+        <v>1995</v>
+      </c>
+      <c r="M32" s="8">
+        <v>2020</v>
+      </c>
+      <c r="N32" s="8">
+        <v>1</v>
+      </c>
+      <c r="O32" s="8">
+        <v>0</v>
+      </c>
+      <c r="P32" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>0</v>
+      </c>
+      <c r="R32" s="8">
+        <v>0</v>
+      </c>
+      <c r="S32" s="8">
+        <v>0</v>
+      </c>
+      <c r="T32" s="8">
+        <v>0</v>
+      </c>
+      <c r="U32" s="8">
+        <v>0</v>
+      </c>
+      <c r="V32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="W32" s="8">
+        <v>0</v>
+      </c>
+      <c r="X32" s="8">
+        <v>0.70789999999999997</v>
+      </c>
+      <c r="Y32" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z32" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC32" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD32" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
@@ -3463,8 +3680,11 @@
   <hyperlinks>
     <hyperlink ref="Y16" r:id="rId1" xr:uid="{57FB1CCF-8A17-4526-B67B-D665DC00480E}"/>
     <hyperlink ref="Y17" r:id="rId2" xr:uid="{4838D400-EECA-4CA6-83E5-1DC8D688795D}"/>
+    <hyperlink ref="Y30" r:id="rId3" xr:uid="{C9C583E0-AAC7-425E-B4C1-C3589760C32D}"/>
+    <hyperlink ref="Y31" r:id="rId4" xr:uid="{7F8CB7A9-A26C-4FF9-A358-6CD716B5C0C1}"/>
+    <hyperlink ref="Y32" r:id="rId5" xr:uid="{D635E882-8399-46A6-B160-868A9DE10672}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additional analysis while documenting The Data for the report
</commit_message>
<xml_diff>
--- a/cs5010_Dict_DRAFTv2_100720.xlsx
+++ b/cs5010_Dict_DRAFTv2_100720.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana McSpadden\Documents\UVaCode\Python\LifeOfBrian-USHousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2718B5F8-1867-4CF8-8801-7FBC92FE3A65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE252C9E-BF75-4402-A164-D1AE47AA1A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="2220" windowWidth="26100" windowHeight="11415" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
+    <workbookView xWindow="9180" yWindow="84" windowWidth="13488" windowHeight="12144" xr2:uid="{C10BA537-74AF-4EA9-9DA5-074E7A0166BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="141">
   <si>
     <t>Source</t>
   </si>
@@ -439,13 +439,31 @@
   </si>
   <si>
     <t>https://www.deptofnumbers.com/rent/virginia/virginia-beach-city/</t>
+  </si>
+  <si>
+    <t>US 30 yr FRM</t>
+  </si>
+  <si>
+    <t>us 30 year FRM mortgage rate</t>
+  </si>
+  <si>
+    <t>http://www.freddiemac.com/pmms/#</t>
+  </si>
+  <si>
+    <t>US 30 yr frm</t>
+  </si>
+  <si>
+    <t>US 15 yr FRM</t>
+  </si>
+  <si>
+    <t>US 5/1 ARM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +492,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -518,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -553,6 +577,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -870,9 +895,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE930BE5-76EF-4DE3-A62A-9FA65577EC5F}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y29" sqref="Y29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3582,41 +3607,105 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="8"/>
-      <c r="AD33" s="8"/>
+    <row r="33" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="8">
+        <v>27</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+      <c r="J33" s="8">
+        <v>0</v>
+      </c>
+      <c r="K33" s="8">
+        <v>1</v>
+      </c>
+      <c r="L33" s="8">
+        <v>1971</v>
+      </c>
+      <c r="M33" s="8">
+        <v>2019</v>
+      </c>
+      <c r="N33" s="8">
+        <v>1</v>
+      </c>
+      <c r="O33" s="8">
+        <v>0</v>
+      </c>
+      <c r="P33" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>0</v>
+      </c>
+      <c r="R33" s="8">
+        <v>0</v>
+      </c>
+      <c r="S33" s="8">
+        <v>0</v>
+      </c>
+      <c r="T33" s="8">
+        <v>0</v>
+      </c>
+      <c r="U33" s="8">
+        <v>0</v>
+      </c>
+      <c r="V33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="W33" s="8">
+        <v>3.31</v>
+      </c>
+      <c r="X33" s="8">
+        <v>18.63</v>
+      </c>
+      <c r="Y33" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA33" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB33" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC33" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD33" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="8">
+        <v>28</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="C34" s="13"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -3647,8 +3736,12 @@
       <c r="AD34" s="8"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
+      <c r="A35" s="8">
+        <v>29</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="C35" s="13"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>

</xml_diff>